<commit_message>
se diseñan formas para pintar el diagrama
</commit_message>
<xml_diff>
--- a/Forma Diagrama.xlsx
+++ b/Forma Diagrama.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="11580"/>
+    <workbookView windowWidth="28800" windowHeight="12030"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -66,10 +66,17 @@
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -590,137 +597,137 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -741,6 +748,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1275,15 +1288,20 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:R11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:L11"/>
+      <selection activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
+  <cols>
+    <col min="15" max="16" width="11.5714285714286" customWidth="1"/>
+    <col min="17" max="17" width="19.1428571428571" customWidth="1"/>
+    <col min="18" max="18" width="10.4285714285714" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:18">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1298,8 +1316,15 @@
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
+      <c r="O1" s="7" t="str">
+        <f>A1</f>
+        <v>Inicio</v>
+      </c>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:18">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="2"/>
@@ -1312,8 +1337,21 @@
       <c r="J2" s="2"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
+      <c r="O2" s="7" t="str">
+        <f>A4</f>
+        <v>Paso 1</v>
+      </c>
+      <c r="P2" s="7"/>
+      <c r="Q2" t="str">
+        <f>E4</f>
+        <v>Datos personales</v>
+      </c>
+      <c r="R2" t="str">
+        <f>I4</f>
+        <v>Paso Final</v>
+      </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:18">
       <c r="A3" s="1"/>
       <c r="B3" s="4"/>
       <c r="C3" s="1"/>
@@ -1326,8 +1364,24 @@
       <c r="J3" s="4"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
+      <c r="O3" t="str">
+        <f>A7</f>
+        <v>Paso 2</v>
+      </c>
+      <c r="P3" s="8" t="str">
+        <f>C7</f>
+        <v>#Paso Final</v>
+      </c>
+      <c r="Q3" t="str">
+        <f>E7</f>
+        <v>Datos personales 1</v>
+      </c>
+      <c r="R3" s="8" t="str">
+        <f>I7</f>
+        <v>#Inicio</v>
+      </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:17">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -1346,8 +1400,16 @@
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
+      <c r="O4" s="8" t="str">
+        <f>A9</f>
+        <v>#Paso Final</v>
+      </c>
+      <c r="Q4" t="str">
+        <f>E9</f>
+        <v>Datos personales 2</v>
+      </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:17">
       <c r="A5" s="1"/>
       <c r="B5" s="4"/>
       <c r="C5" s="1"/>
@@ -1360,6 +1422,10 @@
       <c r="J5" s="4"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
+      <c r="Q5" s="8" t="str">
+        <f>E11</f>
+        <v>#Paso Final</v>
+      </c>
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="1"/>
@@ -1440,8 +1506,10 @@
       <c r="H11" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="13">
     <mergeCell ref="A1:L1"/>
+    <mergeCell ref="O1:R1"/>
+    <mergeCell ref="O2:P2"/>
     <mergeCell ref="A4:D4"/>
     <mergeCell ref="E4:H4"/>
     <mergeCell ref="I4:L4"/>

</xml_diff>